<commit_message>
Tagged 4Q267 frag. 1
</commit_message>
<xml_diff>
--- a/editions/4Q266/457_1926_Frg_1_a/457_1927.xlsx
+++ b/editions/4Q266/457_1926_Frg_1_a/457_1927.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Tucker-James/github/SQE-Damascus/editions/4Q266/457_1926_Frg_1_a/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/External/github/SQE-Damascus/editions/4Q266/457_1926_Frg_1_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEAFF80-9445-734C-88AB-52B3F7015AC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952CFE7B-C2EA-BB4C-B687-15EF9FEC1DC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="poVR+9k3zqxCx69MnAeRPS0K9MfNU+KaOqZ8DZDhFpQsVpmDIuLsEelRgvES3MBx0tToY1quBTUg5EYROKvmEQ==" workbookSaltValue="1lLk6sVdKsislgNF3oz/lw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8920" windowWidth="34440" windowHeight="12680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="10040" windowWidth="34440" windowHeight="12680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHARs" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1219,9 +1222,9 @@
   <dimension ref="A1:Y168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G167" sqref="G167"/>
+      <selection pane="bottomLeft" activeCell="N68" sqref="N68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>